<commit_message>
Change headers to h2 or h2 strapline Resizable input box in facets new color....darker, more contrast. fix entry layout.
git-svn-id: https://svn.code.sf.net/p/metabolomes/code/trunk@1218 71bfadd5-8d58-49b2-b2b0-ff0b8e09f556
</commit_message>
<xml_diff>
--- a/metabolights-webapps/src/main/webapp/var/color-css-generator.xlsx
+++ b/metabolights-webapps/src/main/webapp/var/color-css-generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="28280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Color Scheme" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="293">
   <si>
     <t>/*</t>
   </si>
@@ -825,69 +825,6 @@
     <t>tr.coloured{</t>
   </si>
   <si>
-    <t>#####  Palette URL: http://colorschemedesigner.com/#4362356D1w0w0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #ACAAC5 = rgb(172,170,197)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #868594 = rgb(134,133,148)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #3D3780 = rgb(61,55,128)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #CCCBE2 = rgb(204,203,226)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #D2D1E2 = rgb(210,209,226)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #B5A3C0 = rgb(181,163,192)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #8A7F90 = rgb(138,127,144)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #63357C = rgb(99,53,124)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #D6C6DF = rgb(214,198,223)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #D9CDDF = rgb(217,205,223)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #9CB0B8 = rgb(156,176,184)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #7A868A = rgb(122,134,138)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #336478 = rgb(51,100,120)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #C2D5DB = rgb(194,213,219)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #C9D6DB = rgb(201,214,219)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #FFF6D6 = rgb(255,246,214)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #BFBAA8 = rgb(191,186,168)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #A69046 = rgb(166,144,70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #FFF8E1 = rgb(255,248,225)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #FFFAE9 = rgb(255,250,233)</t>
-  </si>
-  <si>
     <t>.publication{</t>
   </si>
   <si>
@@ -919,6 +856,72 @@
   </si>
   <si>
     <t>div#local-title.logo-title span {margin-top:2em}</t>
+  </si>
+  <si>
+    <t>#####  Palette URL: http://colorschemedesigner.com/#43623gpuDw0w0</t>
+  </si>
+  <si>
+    <t>#####  Color Space: RGB;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #645FAA = rgb(100,95,170)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #58557F = rgb(88,85,127)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #251F6E = rgb(37,31,110)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #938ED5 = rgb(147,142,213)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #A5A1D5 = rgb(165,161,213)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #8754A3 = rgb(135,84,163)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #6A4E7A = rgb(106,78,122)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #4E1B6A = rgb(78,27,106)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #B685D1 = rgb(182,133,209)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #BD99D1 = rgb(189,153,209)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #4E8499 = rgb(78,132,153)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #496773 = rgb(73,103,115)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #194F64 = rgb(25,79,100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #81B7CC = rgb(129,183,204)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #95BDCC = rgb(149,189,204)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #F4D777 = rgb(244,215,119)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #B7A771 = rgb(183,167,113)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #9F8327 = rgb(159,131,39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #FAE49A = rgb(250,228,154)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #FAE9B3 = rgb(250,233,179)</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1038,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1076,6 +1079,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1139,7 +1156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="101">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1206,6 +1223,20 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="18" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1228,7 +1259,28 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1682,18 +1734,18 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="12" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="str">
         <f>A14</f>
-        <v>#####  Palette URL: http://colorschemedesigner.com/#4362356D1w0w0</v>
+        <v>#####  Palette URL: http://colorschemedesigner.com/#43623gpuDw0w0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="12" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1733,87 +1785,87 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ref="B21:B22" si="0">MID(A21,13,7)</f>
-        <v>#ACAAC5</v>
+        <v>#645FAA</v>
       </c>
       <c r="C21" s="2" t="str">
         <f>RIGHT(A21,LEN(A21) -FIND("=",A21,15)+2)</f>
-        <v xml:space="preserve"> = rgb(172,170,197)</v>
+        <v xml:space="preserve"> = rgb(100,95,170)</v>
       </c>
       <c r="D21" s="5" t="str">
         <f>CONCATENATE(LEFT(A21,12),B21,C21)</f>
-        <v xml:space="preserve">   var. 1 = #ACAAC5 = rgb(172,170,197)</v>
+        <v xml:space="preserve">   var. 1 = #645FAA = rgb(100,95,170)</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>#868594</v>
+        <v>#58557F</v>
       </c>
       <c r="C22" s="2" t="str">
         <f t="shared" ref="C22:C25" si="1">RIGHT(A22,LEN(A22) -FIND("=",A22,15)+2)</f>
-        <v xml:space="preserve"> = rgb(134,133,148)</v>
+        <v xml:space="preserve"> = rgb(88,85,127)</v>
       </c>
       <c r="D22" s="5" t="str">
         <f>CONCATENATE(LEFT(A22,12),B22,C22)</f>
-        <v xml:space="preserve">   var. 2 = #868594 = rgb(134,133,148)</v>
+        <v xml:space="preserve">   var. 2 = #58557F = rgb(88,85,127)</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B23" s="2" t="str">
         <f>MID(A23,13,7)</f>
-        <v>#3D3780</v>
+        <v>#251F6E</v>
       </c>
       <c r="C23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(61,55,128)</v>
+        <v xml:space="preserve"> = rgb(37,31,110)</v>
       </c>
       <c r="D23" s="5" t="str">
         <f>CONCATENATE(LEFT(A23,12),B23,C23)</f>
-        <v xml:space="preserve">   var. 3 = #3D3780 = rgb(61,55,128)</v>
+        <v xml:space="preserve">   var. 3 = #251F6E = rgb(37,31,110)</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B24" s="2" t="str">
         <f>MID(A24,13,7)</f>
-        <v>#CCCBE2</v>
+        <v>#938ED5</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(204,203,226)</v>
+        <v xml:space="preserve"> = rgb(147,142,213)</v>
       </c>
       <c r="D24" s="5" t="str">
         <f>CONCATENATE(LEFT(A24,12),B24,C24)</f>
-        <v xml:space="preserve">   var. 4 = #CCCBE2 = rgb(204,203,226)</v>
+        <v xml:space="preserve">   var. 4 = #938ED5 = rgb(147,142,213)</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="B25" s="2" t="str">
         <f>MID(A25,13,7)</f>
-        <v>#D2D1E2</v>
+        <v>#A5A1D5</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(210,209,226)</v>
+        <v xml:space="preserve"> = rgb(165,161,213)</v>
       </c>
       <c r="D25" s="5" t="str">
         <f>CONCATENATE(LEFT(A25,12),B25,C25)</f>
-        <v xml:space="preserve">   var. 5 = #D2D1E2 = rgb(210,209,226)</v>
+        <v xml:space="preserve">   var. 5 = #A5A1D5 = rgb(165,161,213)</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1838,87 +1890,87 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B29" s="2" t="str">
         <f>MID(A29,13,7)</f>
-        <v>#B5A3C0</v>
+        <v>#8754A3</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" ref="C29:C49" si="2">RIGHT(A29,LEN(A29) -FIND("=",A29,15)+2)</f>
-        <v xml:space="preserve"> = rgb(181,163,192)</v>
+        <v xml:space="preserve"> = rgb(135,84,163)</v>
       </c>
       <c r="D29" s="5" t="str">
         <f>CONCATENATE(LEFT(A29,12),B29,C29)</f>
-        <v xml:space="preserve">   var. 1 = #B5A3C0 = rgb(181,163,192)</v>
+        <v xml:space="preserve">   var. 1 = #8754A3 = rgb(135,84,163)</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="B30" s="2" t="str">
         <f>MID(A30,13,7)</f>
-        <v>#8A7F90</v>
+        <v>#6A4E7A</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(138,127,144)</v>
+        <v xml:space="preserve"> = rgb(106,78,122)</v>
       </c>
       <c r="D30" s="5" t="str">
         <f>CONCATENATE(LEFT(A30,12),B30,C30)</f>
-        <v xml:space="preserve">   var. 2 = #8A7F90 = rgb(138,127,144)</v>
+        <v xml:space="preserve">   var. 2 = #6A4E7A = rgb(106,78,122)</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B31" s="2" t="str">
         <f>MID(A31,13,7)</f>
-        <v>#63357C</v>
+        <v>#4E1B6A</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(99,53,124)</v>
+        <v xml:space="preserve"> = rgb(78,27,106)</v>
       </c>
       <c r="D31" s="5" t="str">
         <f>CONCATENATE(LEFT(A31,12),B31,C31)</f>
-        <v xml:space="preserve">   var. 3 = #63357C = rgb(99,53,124)</v>
+        <v xml:space="preserve">   var. 3 = #4E1B6A = rgb(78,27,106)</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="12" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B32" s="2" t="str">
         <f>MID(A32,13,7)</f>
-        <v>#D6C6DF</v>
+        <v>#B685D1</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(214,198,223)</v>
+        <v xml:space="preserve"> = rgb(182,133,209)</v>
       </c>
       <c r="D32" s="5" t="str">
         <f>CONCATENATE(LEFT(A32,12),B32,C32)</f>
-        <v xml:space="preserve">   var. 4 = #D6C6DF = rgb(214,198,223)</v>
+        <v xml:space="preserve">   var. 4 = #B685D1 = rgb(182,133,209)</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="12" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B33" s="2" t="str">
         <f>MID(A33,13,7)</f>
-        <v>#D9CDDF</v>
+        <v>#BD99D1</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(217,205,223)</v>
+        <v xml:space="preserve"> = rgb(189,153,209)</v>
       </c>
       <c r="D33" s="5" t="str">
         <f>CONCATENATE(LEFT(A33,12),B33,C33)</f>
-        <v xml:space="preserve">   var. 5 = #D9CDDF = rgb(217,205,223)</v>
+        <v xml:space="preserve">   var. 5 = #BD99D1 = rgb(189,153,209)</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1943,87 +1995,87 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="B37" s="2" t="str">
         <f>MID(A37,13,7)</f>
-        <v>#9CB0B8</v>
+        <v>#4E8499</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" ref="C37" si="3">RIGHT(A37,LEN(A37) -FIND("=",A37,15)+2)</f>
-        <v xml:space="preserve"> = rgb(156,176,184)</v>
+        <v xml:space="preserve"> = rgb(78,132,153)</v>
       </c>
       <c r="D37" s="5" t="str">
         <f>CONCATENATE(LEFT(A37,12),B37,C37)</f>
-        <v xml:space="preserve">   var. 1 = #9CB0B8 = rgb(156,176,184)</v>
+        <v xml:space="preserve">   var. 1 = #4E8499 = rgb(78,132,153)</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B38" s="2" t="str">
         <f>MID(A38,13,7)</f>
-        <v>#7A868A</v>
+        <v>#496773</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(122,134,138)</v>
+        <v xml:space="preserve"> = rgb(73,103,115)</v>
       </c>
       <c r="D38" s="5" t="str">
         <f>CONCATENATE(LEFT(A38,12),B38,C38)</f>
-        <v xml:space="preserve">   var. 2 = #7A868A = rgb(122,134,138)</v>
+        <v xml:space="preserve">   var. 2 = #496773 = rgb(73,103,115)</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="12" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="B39" s="2" t="str">
         <f>MID(A39,13,7)</f>
-        <v>#336478</v>
+        <v>#194F64</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(51,100,120)</v>
+        <v xml:space="preserve"> = rgb(25,79,100)</v>
       </c>
       <c r="D39" s="5" t="str">
         <f>CONCATENATE(LEFT(A39,12),B39,C39)</f>
-        <v xml:space="preserve">   var. 3 = #336478 = rgb(51,100,120)</v>
+        <v xml:space="preserve">   var. 3 = #194F64 = rgb(25,79,100)</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="12" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B40" s="2" t="str">
         <f>MID(A40,13,7)</f>
-        <v>#C2D5DB</v>
+        <v>#81B7CC</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(194,213,219)</v>
+        <v xml:space="preserve"> = rgb(129,183,204)</v>
       </c>
       <c r="D40" s="5" t="str">
         <f>CONCATENATE(LEFT(A40,12),B40,C40)</f>
-        <v xml:space="preserve">   var. 4 = #C2D5DB = rgb(194,213,219)</v>
+        <v xml:space="preserve">   var. 4 = #81B7CC = rgb(129,183,204)</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B41" s="2" t="str">
         <f>MID(A41,13,7)</f>
-        <v>#C9D6DB</v>
+        <v>#95BDCC</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(201,214,219)</v>
+        <v xml:space="preserve"> = rgb(149,189,204)</v>
       </c>
       <c r="D41" s="5" t="str">
         <f>CONCATENATE(LEFT(A41,12),B41,C41)</f>
-        <v xml:space="preserve">   var. 5 = #C9D6DB = rgb(201,214,219)</v>
+        <v xml:space="preserve">   var. 5 = #95BDCC = rgb(149,189,204)</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2048,87 +2100,87 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B45" s="2" t="str">
         <f>MID(A45,13,7)</f>
-        <v>#FFF6D6</v>
+        <v>#F4D777</v>
       </c>
       <c r="C45" s="2" t="str">
         <f t="shared" ref="C45" si="4">RIGHT(A45,LEN(A45) -FIND("=",A45,15)+2)</f>
-        <v xml:space="preserve"> = rgb(255,246,214)</v>
+        <v xml:space="preserve"> = rgb(244,215,119)</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>CONCATENATE(LEFT(A45,12),B45,C45)</f>
-        <v xml:space="preserve">   var. 1 = #FFF6D6 = rgb(255,246,214)</v>
+        <v xml:space="preserve">   var. 1 = #F4D777 = rgb(244,215,119)</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="12" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="B46" s="2" t="str">
         <f>MID(A46,13,7)</f>
-        <v>#BFBAA8</v>
+        <v>#B7A771</v>
       </c>
       <c r="C46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(191,186,168)</v>
+        <v xml:space="preserve"> = rgb(183,167,113)</v>
       </c>
       <c r="D46" s="5" t="str">
         <f>CONCATENATE(LEFT(A46,12),B46,C46)</f>
-        <v xml:space="preserve">   var. 2 = #BFBAA8 = rgb(191,186,168)</v>
+        <v xml:space="preserve">   var. 2 = #B7A771 = rgb(183,167,113)</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="12" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B47" s="2" t="str">
         <f>MID(A47,13,7)</f>
-        <v>#A69046</v>
+        <v>#9F8327</v>
       </c>
       <c r="C47" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(166,144,70)</v>
+        <v xml:space="preserve"> = rgb(159,131,39)</v>
       </c>
       <c r="D47" s="5" t="str">
         <f>CONCATENATE(LEFT(A47,12),B47,C47)</f>
-        <v xml:space="preserve">   var. 3 = #A69046 = rgb(166,144,70)</v>
+        <v xml:space="preserve">   var. 3 = #9F8327 = rgb(159,131,39)</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="12" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="B48" s="2" t="str">
         <f>MID(A48,13,7)</f>
-        <v>#FFF8E1</v>
+        <v>#FAE49A</v>
       </c>
       <c r="C48" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(255,248,225)</v>
+        <v xml:space="preserve"> = rgb(250,228,154)</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>CONCATENATE(LEFT(A48,12),B48,C48)</f>
-        <v xml:space="preserve">   var. 4 = #FFF8E1 = rgb(255,248,225)</v>
+        <v xml:space="preserve">   var. 4 = #FAE49A = rgb(250,228,154)</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="12" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B49" s="2" t="str">
         <f>MID(A49,13,7)</f>
-        <v>#FFFAE9</v>
+        <v>#FAE9B3</v>
       </c>
       <c r="C49" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(255,250,233)</v>
+        <v xml:space="preserve"> = rgb(250,233,179)</v>
       </c>
       <c r="D49" s="5" t="str">
         <f>CONCATENATE(LEFT(A49,12),B49,C49)</f>
-        <v xml:space="preserve">   var. 5 = #FFFAE9 = rgb(255,250,233)</v>
+        <v xml:space="preserve">   var. 5 = #FAE9B3 = rgb(250,233,179)</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2243,7 +2295,7 @@
       <c r="C65" s="2"/>
       <c r="D65" s="5" t="str">
         <f>CONCATENATE("a:visited { border-bottom-color: ", B21,"; }")</f>
-        <v>a:visited { border-bottom-color: #ACAAC5; }</v>
+        <v>a:visited { border-bottom-color: #645FAA; }</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2282,7 +2334,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="5" t="str">
         <f>CONCATENATE("  color: ", B21,";")</f>
-        <v xml:space="preserve">  color: #ACAAC5;</v>
+        <v xml:space="preserve">  color: #645FAA;</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2291,7 +2343,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="5" t="str">
         <f>CONCATENATE("  border-bottom: 1px solid ",B21,";")</f>
-        <v xml:space="preserve">  border-bottom: 1px solid #ACAAC5;</v>
+        <v xml:space="preserve">  border-bottom: 1px solid #645FAA;</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2332,14 +2384,14 @@
       <c r="A77" s="2"/>
       <c r="D77" s="5" t="str">
         <f>CONCATENATE("        color:",B21,";")</f>
-        <v xml:space="preserve">        color:#ACAAC5;</v>
+        <v xml:space="preserve">        color:#645FAA;</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2"/>
       <c r="D78" s="5" t="str">
         <f>CONCATENATE("        border-bottom: 3px double ", B21,";")</f>
-        <v xml:space="preserve">        border-bottom: 3px double #ACAAC5;</v>
+        <v xml:space="preserve">        border-bottom: 3px double #645FAA;</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2360,7 +2412,7 @@
       <c r="A82" s="2"/>
       <c r="D82" s="5" t="str">
         <f>CONCATENATE("a:link { color: ", B31,"; }")</f>
-        <v>a:link { color: #63357C; }</v>
+        <v>a:link { color: #4E1B6A; }</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2383,7 +2435,7 @@
       <c r="A86" s="2"/>
       <c r="D86" s="5" t="str">
         <f>CONCATENATE("a:active { color: ", B39,"; }")</f>
-        <v>a:active { color: #336478; }</v>
+        <v>a:active { color: #194F64; }</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2394,7 +2446,7 @@
       <c r="A88" s="2"/>
       <c r="D88" s="5" t="str">
         <f>CONCATENATE("a.special { background-color: ",B41,"; }")</f>
-        <v>a.special { background-color: #C9D6DB; }</v>
+        <v>a.special { background-color: #95BDCC; }</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2425,7 +2477,7 @@
       <c r="A94" s="2"/>
       <c r="D94" s="5" t="str">
         <f>CONCATENATE("h1 { color: ",B21,"; }")</f>
-        <v>h1 { color: #ACAAC5; }</v>
+        <v>h1 { color: #645FAA; }</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2436,7 +2488,7 @@
       <c r="A96" s="2"/>
       <c r="D96" s="5" t="str">
         <f>CONCATENATE("h2 { color: ", B46,"; }")</f>
-        <v>h2 { color: #BFBAA8; }</v>
+        <v>h2 { color: #B7A771; }</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2519,7 +2571,7 @@
       <c r="A110" s="2"/>
       <c r="D110" s="5" t="str">
         <f>CONCATENATE("        border-bottom-color: ", B21,";")</f>
-        <v xml:space="preserve">        border-bottom-color: #ACAAC5;</v>
+        <v xml:space="preserve">        border-bottom-color: #645FAA;</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2545,8 +2597,8 @@
     <row r="115" spans="1:5">
       <c r="A115" s="2"/>
       <c r="D115" s="5" t="str">
-        <f>CONCATENATE("th { background-color: ", B37,"; }")</f>
-        <v>th { background-color: #9CB0B8; }</v>
+        <f>CONCATENATE("th { background-color: ", Primary5,"; }")</f>
+        <v>th { background-color: #A5A1D5; }</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2577,7 +2629,7 @@
       <c r="A120" s="2"/>
       <c r="D120" s="5" t="str">
         <f>CONCATENATE("border-color: ", B22,"; /* P2 */")</f>
-        <v>border-color: #868594; /* P2 */</v>
+        <v>border-color: #58557F; /* P2 */</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>43</v>
@@ -2587,7 +2639,7 @@
       <c r="A121" s="2"/>
       <c r="D121" s="5" t="str">
         <f>CONCATENATE("background-color: ", B21,"; /* colour P1 */")</f>
-        <v>background-color: #ACAAC5; /* colour P1 */</v>
+        <v>background-color: #645FAA; /* colour P1 */</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>44</v>
@@ -2597,55 +2649,55 @@
       <c r="A122" s="2"/>
       <c r="D122" s="5" t="str">
         <f>CONCATENATE("background-image: -moz-linear-gradient(top, ",B24," , ", B21, ");")</f>
-        <v>background-image: -moz-linear-gradient(top, #CCCBE2 , #ACAAC5);</v>
+        <v>background-image: -moz-linear-gradient(top, #938ED5 , #645FAA);</v>
       </c>
       <c r="E122" s="1" t="str">
         <f>CONCATENATE("    text-shadow: ",B23," 1px 1px;")</f>
-        <v xml:space="preserve">    text-shadow: #3D3780 1px 1px;</v>
+        <v xml:space="preserve">    text-shadow: #251F6E 1px 1px;</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="16">
       <c r="A123" s="2"/>
       <c r="D123" s="5" t="str">
         <f>CONCATENATE("background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, ", B24, "),color-stop(1, ", B21,"));")</f>
-        <v>background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #CCCBE2),color-stop(1, #ACAAC5));</v>
+        <v>background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #938ED5),color-stop(1, #645FAA));</v>
       </c>
       <c r="E123" s="1" t="str">
         <f>CONCATENATE("    border-top: 1px solid ", B25,"; ")</f>
-        <v xml:space="preserve">    border-top: 1px solid #D2D1E2; </v>
+        <v xml:space="preserve">    border-top: 1px solid #A5A1D5; </v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="16">
       <c r="A124" s="2"/>
       <c r="D124" s="5" t="str">
         <f>CONCATENATE("background-image: -webkit-linear-gradient(", B24,", ", B21,");")</f>
-        <v>background-image: -webkit-linear-gradient(#CCCBE2, #ACAAC5);</v>
+        <v>background-image: -webkit-linear-gradient(#938ED5, #645FAA);</v>
       </c>
       <c r="E124" s="1" t="str">
         <f>CONCATENATE("    border-left: 1px solid ",B25,";")</f>
-        <v xml:space="preserve">    border-left: 1px solid #D2D1E2;</v>
+        <v xml:space="preserve">    border-left: 1px solid #A5A1D5;</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="16">
       <c r="A125" s="2"/>
       <c r="D125" s="5" t="str">
         <f>CONCATENATE("background-image: linear-gradient(top, ", B24,", ", B21,");")</f>
-        <v>background-image: linear-gradient(top, #CCCBE2, #ACAAC5);</v>
+        <v>background-image: linear-gradient(top, #938ED5, #645FAA);</v>
       </c>
       <c r="E125" s="1" t="str">
         <f>CONCATENATE("    border-right: 1px solid ", B23,";")</f>
-        <v xml:space="preserve">    border-right: 1px solid #3D3780;</v>
+        <v xml:space="preserve">    border-right: 1px solid #251F6E;</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="16">
       <c r="A126" s="2"/>
       <c r="D126" s="5" t="str">
         <f>CONCATENATE("filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='", B24, "', EndColorStr='", B21,"');")</f>
-        <v>filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#CCCBE2', EndColorStr='#ACAAC5');</v>
+        <v>filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#938ED5', EndColorStr='#645FAA');</v>
       </c>
       <c r="E126" s="1" t="str">
         <f>CONCATENATE("    border-bottom: 1px solid ",B23,";")</f>
-        <v xml:space="preserve">    border-bottom: 1px solid #3D3780;</v>
+        <v xml:space="preserve">    border-bottom: 1px solid #251F6E;</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="16">
@@ -2664,7 +2716,7 @@
       </c>
       <c r="E128" s="1" t="str">
         <f>CONCATENATE("        background-image: -moz-linear-gradient(top, ", B21,", ",B22,");")</f>
-        <v xml:space="preserve">        background-image: -moz-linear-gradient(top, #ACAAC5, #868594);</v>
+        <v xml:space="preserve">        background-image: -moz-linear-gradient(top, #645FAA, #58557F);</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="16">
@@ -2674,7 +2726,7 @@
       </c>
       <c r="E129" s="1" t="str">
         <f>CONCATENATE("    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, ",B22,"));")</f>
-        <v xml:space="preserve">    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, #868594));</v>
+        <v xml:space="preserve">    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, #58557F));</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="16">
@@ -2682,7 +2734,7 @@
       <c r="D130" s="5"/>
       <c r="E130" s="1" t="str">
         <f>CONCATENATE("    background-image: -webkit-linear-gradient(",B21,", ",B22,");" )</f>
-        <v xml:space="preserve">    background-image: -webkit-linear-gradient(#ACAAC5, #868594);</v>
+        <v xml:space="preserve">    background-image: -webkit-linear-gradient(#645FAA, #58557F);</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="16">
@@ -2692,7 +2744,7 @@
       </c>
       <c r="E131" s="1" t="str">
         <f>CONCATENATE("    background-image: linear-gradient(top, ", B21, ", ", B22, ");")</f>
-        <v xml:space="preserve">    background-image: linear-gradient(top, #ACAAC5, #868594);</v>
+        <v xml:space="preserve">    background-image: linear-gradient(top, #645FAA, #58557F);</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="16">
@@ -2702,14 +2754,14 @@
       </c>
       <c r="E132" s="1" t="str">
         <f>CONCATENATE("    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='", B21, "', EndColorStr='", B22,"');")</f>
-        <v xml:space="preserve">    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#ACAAC5', EndColorStr='#868594');</v>
+        <v xml:space="preserve">    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#645FAA', EndColorStr='#58557F');</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="16">
       <c r="A133" s="2"/>
       <c r="D133" s="5" t="str">
         <f>CONCATENATE("form input.submit:active { background: ", B21,"; }")</f>
-        <v>form input.submit:active { background: #ACAAC5; }</v>
+        <v>form input.submit:active { background: #645FAA; }</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>22</v>
@@ -2723,7 +2775,7 @@
       <c r="A135" s="2"/>
       <c r="D135" s="5" t="str">
         <f>CONCATENATE("div.box { border: 10px solid ", SECB5,"; }")</f>
-        <v>div.box { border: 10px solid #C9D6DB; }</v>
+        <v>div.box { border: 10px solid #95BDCC; }</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>46</v>
@@ -2734,14 +2786,14 @@
       <c r="D136" s="5"/>
       <c r="E136" s="1" t="str">
         <f>CONCATENATE("div#local-masthead { background-color: ", B25, "; }")</f>
-        <v>div#local-masthead { background-color: #D2D1E2; }</v>
+        <v>div#local-masthead { background-color: #A5A1D5; }</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="2"/>
       <c r="D137" s="5" t="str">
         <f>CONCATENATE("div#local-masthead { background-color: ", B25,"; }")</f>
-        <v>div#local-masthead { background-color: #D2D1E2; }</v>
+        <v>div#local-masthead { background-color: #A5A1D5; }</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="16">
@@ -2785,14 +2837,14 @@
       </c>
       <c r="E142" s="1" t="str">
         <f>CONCATENATE("border-bottom: 3px solid ", B21, ";")</f>
-        <v>border-bottom: 3px solid #ACAAC5;</v>
+        <v>border-bottom: 3px solid #645FAA;</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="16">
       <c r="A143" s="2"/>
       <c r="D143" s="5" t="str">
         <f>CONCATENATE("border-bottom: 3px solid ", Primary1, ";")</f>
-        <v>border-bottom: 3px solid #ACAAC5;</v>
+        <v>border-bottom: 3px solid #645FAA;</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>22</v>
@@ -2905,14 +2957,14 @@
       <c r="A162" s="2"/>
       <c r="D162" s="5" t="str">
         <f>CONCATENATE(".primary-1 { background-color: ", Primary1,"}")</f>
-        <v>.primary-1 { background-color: #ACAAC5}</v>
+        <v>.primary-1 { background-color: #645FAA}</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="2"/>
       <c r="D163" s="5" t="str">
         <f>CONCATENATE(".primary-2 { background-color: ", Primary2,"}")</f>
-        <v>.primary-2 { background-color: #868594}</v>
+        <v>.primary-2 { background-color: #58557F}</v>
       </c>
       <c r="E163" s="3"/>
     </row>
@@ -2920,7 +2972,7 @@
       <c r="A164" s="2"/>
       <c r="D164" s="5" t="str">
         <f>CONCATENATE(".primary-3 { background-color: ", Primary3,"}")</f>
-        <v>.primary-3 { background-color: #3D3780}</v>
+        <v>.primary-3 { background-color: #251F6E}</v>
       </c>
       <c r="E164" s="3"/>
     </row>
@@ -2928,7 +2980,7 @@
       <c r="A165" s="2"/>
       <c r="D165" s="5" t="str">
         <f>CONCATENATE(".primary-4 { background-color: ", Primary4,"}")</f>
-        <v>.primary-4 { background-color: #CCCBE2}</v>
+        <v>.primary-4 { background-color: #938ED5}</v>
       </c>
       <c r="E165" s="3"/>
     </row>
@@ -2936,7 +2988,7 @@
       <c r="A166" s="2"/>
       <c r="D166" s="5" t="str">
         <f>CONCATENATE(".primary-5 { background-color: ", Primary5,"}")</f>
-        <v>.primary-5 { background-color: #D2D1E2}</v>
+        <v>.primary-5 { background-color: #A5A1D5}</v>
       </c>
       <c r="E166" s="3"/>
     </row>
@@ -2949,14 +3001,14 @@
       <c r="A168" s="2"/>
       <c r="D168" s="5" t="str">
         <f>CONCATENATE(".secondary-a-1 { background-color: ", SECA1,"}")</f>
-        <v>.secondary-a-1 { background-color: #B5A3C0}</v>
+        <v>.secondary-a-1 { background-color: #8754A3}</v>
       </c>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="2"/>
       <c r="D169" s="5" t="str">
         <f>CONCATENATE(".secondary-a-2 { background-color: ", SECA2,"}")</f>
-        <v>.secondary-a-2 { background-color: #8A7F90}</v>
+        <v>.secondary-a-2 { background-color: #6A4E7A}</v>
       </c>
       <c r="E169" s="4"/>
     </row>
@@ -2964,21 +3016,21 @@
       <c r="A170" s="2"/>
       <c r="D170" s="5" t="str">
         <f>CONCATENATE(".secondary-a-3 { background-color: ", SECA3,"}")</f>
-        <v>.secondary-a-3 { background-color: #63357C}</v>
+        <v>.secondary-a-3 { background-color: #4E1B6A}</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="2"/>
       <c r="D171" s="5" t="str">
         <f>CONCATENATE(".secondary-a-4 { background-color: ", SECA4,"}")</f>
-        <v>.secondary-a-4 { background-color: #D6C6DF}</v>
+        <v>.secondary-a-4 { background-color: #B685D1}</v>
       </c>
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="2"/>
       <c r="D172" s="5" t="str">
         <f>CONCATENATE(".secondary-a-5 { background-color: ", SECA5,"}")</f>
-        <v>.secondary-a-5 { background-color: #D9CDDF}</v>
+        <v>.secondary-a-5 { background-color: #BD99D1}</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -2989,35 +3041,35 @@
       <c r="A174" s="2"/>
       <c r="D174" s="5" t="str">
         <f>CONCATENATE(".secondary-b-1 { background-color: ", SECB1,"}")</f>
-        <v>.secondary-b-1 { background-color: #9CB0B8}</v>
+        <v>.secondary-b-1 { background-color: #4E8499}</v>
       </c>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="2"/>
       <c r="D175" s="5" t="str">
         <f>CONCATENATE(".secondary-b-2 { background-color: ", SECB2,"}")</f>
-        <v>.secondary-b-2 { background-color: #7A868A}</v>
+        <v>.secondary-b-2 { background-color: #496773}</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="2"/>
       <c r="D176" s="5" t="str">
         <f>CONCATENATE(".secondary-b-3 { background-color: ", SECB3,"}")</f>
-        <v>.secondary-b-3 { background-color: #336478}</v>
+        <v>.secondary-b-3 { background-color: #194F64}</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="2"/>
       <c r="D177" s="5" t="str">
         <f>CONCATENATE(".secondary-b-4 { background-color: ", SECB4,"}")</f>
-        <v>.secondary-b-4 { background-color: #C2D5DB}</v>
+        <v>.secondary-b-4 { background-color: #81B7CC}</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="2"/>
       <c r="D178" s="5" t="str">
         <f>CONCATENATE(".secondary-b-5 { background-color: ", SECB5,"}")</f>
-        <v>.secondary-b-5 { background-color: #C9D6DB}</v>
+        <v>.secondary-b-5 { background-color: #95BDCC}</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3028,35 +3080,35 @@
       <c r="A180" s="2"/>
       <c r="D180" s="5" t="str">
         <f>CONCATENATE(".complement-1 { background-color: ", COMP1,"}")</f>
-        <v>.complement-1 { background-color: #FFF6D6}</v>
+        <v>.complement-1 { background-color: #F4D777}</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="2"/>
       <c r="D181" s="5" t="str">
         <f>CONCATENATE(".complement-2 { background-color: ", COMP2,"}")</f>
-        <v>.complement-2 { background-color: #BFBAA8}</v>
+        <v>.complement-2 { background-color: #B7A771}</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="2"/>
       <c r="D182" s="5" t="str">
         <f>CONCATENATE(".complement-3 { background-color: ", COMP3,"}")</f>
-        <v>.complement-3 { background-color: #A69046}</v>
+        <v>.complement-3 { background-color: #9F8327}</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="2"/>
       <c r="D183" s="5" t="str">
         <f>CONCATENATE(".complement-4 { background-color: ", COMP4,"}")</f>
-        <v>.complement-4 { background-color: #FFF8E1}</v>
+        <v>.complement-4 { background-color: #FAE49A}</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="2"/>
       <c r="D184" s="5" t="str">
         <f>CONCATENATE(".complement-5 { background-color: ", COMP5,"}")</f>
-        <v>.complement-5 { background-color: #FFFAE9}</v>
+        <v>.complement-5 { background-color: #FAE9B3}</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3087,13 +3139,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C340"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="25.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3173,7 +3227,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3541,14 +3595,14 @@
       <c r="A85" s="9"/>
       <c r="B85" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #3D3780;</v>
+        <v>color: #251F6E;</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="9"/>
       <c r="B86" s="9" t="str">
-        <f>CONCATENATE("background: ", Primary1,";")</f>
-        <v>background: #ACAAC5;</v>
+        <f>CONCATENATE("background: ", Primary4,";")</f>
+        <v>background: #938ED5;</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3822,7 +3876,7 @@
     <row r="149" spans="1:2">
       <c r="B149" s="7" t="str">
         <f>CONCATENATE("color:",COMP1,";")</f>
-        <v>color:#FFF6D6;</v>
+        <v>color:#F4D777;</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -3848,7 +3902,7 @@
     <row r="155" spans="1:2">
       <c r="B155" s="7" t="str">
         <f>CONCATENATE("background-color:", COMP1,";")</f>
-        <v>background-color:#FFF6D6;</v>
+        <v>background-color:#F4D777;</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -3864,7 +3918,7 @@
     <row r="159" spans="1:2">
       <c r="B159" s="7" t="str">
         <f>CONCATENATE("color:", SECB1, ";")</f>
-        <v>color:#9CB0B8;</v>
+        <v>color:#4E8499;</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -3885,7 +3939,7 @@
     <row r="164" spans="1:2">
       <c r="B164" s="7" t="str">
         <f>CONCATENATE("background-color:", SECB1, ";")</f>
-        <v>background-color:#9CB0B8;</v>
+        <v>background-color:#4E8499;</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -4171,7 +4225,7 @@
     <row r="231" spans="1:2">
       <c r="B231" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #3D3780;</v>
+        <v>color: #251F6E;</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -4212,7 +4266,7 @@
     <row r="240" spans="1:2">
       <c r="B240" s="7" t="str">
         <f>CONCATENATE("color: ", COMP3,";")</f>
-        <v>color: #A69046;</v>
+        <v>color: #9F8327;</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -4248,7 +4302,7 @@
     <row r="248" spans="1:2">
       <c r="B248" s="7" t="str">
         <f>CONCATENATE("border: 1px solid ", Primary3)</f>
-        <v>border: 1px solid #3D3780</v>
+        <v>border: 1px solid #251F6E</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -4304,7 +4358,7 @@
     <row r="260" spans="1:2">
       <c r="B260" s="7" t="str">
         <f>CONCATENATE("background: ", Primary5, ";")</f>
-        <v>background: #D2D1E2;</v>
+        <v>background: #A5A1D5;</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -4330,13 +4384,13 @@
     <row r="266" spans="1:2">
       <c r="B266" s="7" t="str">
         <f>CONCATENATE("background: ", Primary4, ";")</f>
-        <v>background: #CCCBE2;</v>
+        <v>background: #938ED5;</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="B267" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #3D3780;</v>
+        <v>color: #251F6E;</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -4372,7 +4426,7 @@
     <row r="275" spans="1:2">
       <c r="B275" s="7" t="str">
         <f>CONCATENATE("border-top-color:", COMP3,";")</f>
-        <v>border-top-color:#A69046;</v>
+        <v>border-top-color:#9F8327;</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -4577,8 +4631,8 @@
     </row>
     <row r="324" spans="1:2">
       <c r="B324" s="7" t="str">
-        <f>CONCATENATE("background: ", SECB4,";")</f>
-        <v>background: #C2D5DB;</v>
+        <f>CONCATENATE("background: ", Primary2,";")</f>
+        <v>background: #58557F;</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -4588,32 +4642,32 @@
     </row>
     <row r="327" spans="1:2">
       <c r="A327" s="7" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="7" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329" s="7" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="7" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="7" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332" s="7" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -4623,12 +4677,12 @@
     </row>
     <row r="334" spans="1:2">
       <c r="A334" s="7" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="7" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -4638,12 +4692,12 @@
     </row>
     <row r="338" spans="1:1">
       <c r="A338" s="7" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" s="7" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
     </row>
     <row r="340" spans="1:1">
@@ -4653,6 +4707,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="J1:J340">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Change color again! Home page title alignment Contact us navigation item Icons changed (for Download studies and download software) Alternative rows colour changed (to a grey-ish).
git-svn-id: https://svn.code.sf.net/p/metabolomes/code/trunk@1221 71bfadd5-8d58-49b2-b2b0-ff0b8e09f556
</commit_message>
<xml_diff>
--- a/metabolights-webapps/src/main/webapp/var/color-css-generator.xlsx
+++ b/metabolights-webapps/src/main/webapp/var/color-css-generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8360" yWindow="2920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Color Scheme" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="COMP3">'Color Scheme'!$B$47</definedName>
     <definedName name="COMP4">'Color Scheme'!$B$48</definedName>
     <definedName name="COMP5">'Color Scheme'!$B$49</definedName>
-    <definedName name="OutputCSS">'Color Scheme'!$D$1:$D$186</definedName>
+    <definedName name="OutputCSS">'Color Scheme'!$D$1:$D$196</definedName>
     <definedName name="Primary1">'Color Scheme'!$B$21</definedName>
     <definedName name="Primary2">'Color Scheme'!$B$22</definedName>
     <definedName name="Primary3">'Color Scheme'!$B$23</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="295">
   <si>
     <t>/*</t>
   </si>
@@ -858,70 +858,76 @@
     <t>div#local-title.logo-title span {margin-top:2em}</t>
   </si>
   <si>
-    <t>#####  Palette URL: http://colorschemedesigner.com/#43623gpuDw0w0</t>
-  </si>
-  <si>
-    <t>#####  Color Space: RGB;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #645FAA = rgb(100,95,170)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #58557F = rgb(88,85,127)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #251F6E = rgb(37,31,110)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #938ED5 = rgb(147,142,213)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #A5A1D5 = rgb(165,161,213)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #8754A3 = rgb(135,84,163)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #6A4E7A = rgb(106,78,122)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #4E1B6A = rgb(78,27,106)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #B685D1 = rgb(182,133,209)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #BD99D1 = rgb(189,153,209)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #4E8499 = rgb(78,132,153)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #496773 = rgb(73,103,115)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #194F64 = rgb(25,79,100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #81B7CC = rgb(129,183,204)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #95BDCC = rgb(149,189,204)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 1 = #F4D777 = rgb(244,215,119)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 2 = #B7A771 = rgb(183,167,113)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 3 = #9F8327 = rgb(159,131,39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 4 = #FAE49A = rgb(250,228,154)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   var. 5 = #FAE9B3 = rgb(250,233,179)</t>
+    <t>#####  Palette URL: http://colorschemedesigner.com/#0.623juoMw0w0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #C58A4D = rgb(197,138,77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #947350 = rgb(148,115,80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #804D19 = rgb(128,77,25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #E2AF7B = rgb(226,175,123)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #E2BD97 = rgb(226,189,151)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #C5A94D = rgb(197,169,77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #948450 = rgb(148,132,80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #806819 = rgb(128,104,25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #E2C97B = rgb(226,201,123)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #E2D097 = rgb(226,208,151)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #BD4A58 = rgb(189,74,88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #8E4D55 = rgb(142,77,85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #7B1824 = rgb(123,24,36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #DE7985 = rgb(222,121,133)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #DE949D = rgb(222,148,157)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 1 = #336B7B = rgb(51,107,123)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 2 = #33535C = rgb(51,83,92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 3 = #104250 = rgb(16,66,80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 4 = #6AABBD = rgb(106,171,189)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   var. 5 = #80AFBD = rgb(128,175,189)</t>
+  </si>
+  <si>
+    <t>div#local-masthead {</t>
+  </si>
+  <si>
+    <t>th a.icon-functional::before{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    color: #ffffff;</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1044,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1079,6 +1085,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1156,7 +1178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="117">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1237,6 +1259,22 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="18" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1259,17 +1297,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1607,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView showGridLines="0" topLeftCell="B134" workbookViewId="0">
+      <selection activeCell="D134" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1740,12 +1768,12 @@
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="str">
         <f>A14</f>
-        <v>#####  Palette URL: http://colorschemedesigner.com/#43623gpuDw0w0</v>
+        <v>#####  Palette URL: http://colorschemedesigner.com/#0.623juoMw0w0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="12" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1785,87 +1813,87 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" ref="B21:B22" si="0">MID(A21,13,7)</f>
-        <v>#645FAA</v>
+        <v>#C58A4D</v>
       </c>
       <c r="C21" s="2" t="str">
         <f>RIGHT(A21,LEN(A21) -FIND("=",A21,15)+2)</f>
-        <v xml:space="preserve"> = rgb(100,95,170)</v>
+        <v xml:space="preserve"> = rgb(197,138,77)</v>
       </c>
       <c r="D21" s="5" t="str">
         <f>CONCATENATE(LEFT(A21,12),B21,C21)</f>
-        <v xml:space="preserve">   var. 1 = #645FAA = rgb(100,95,170)</v>
+        <v xml:space="preserve">   var. 1 = #C58A4D = rgb(197,138,77)</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>#58557F</v>
+        <v>#947350</v>
       </c>
       <c r="C22" s="2" t="str">
         <f t="shared" ref="C22:C25" si="1">RIGHT(A22,LEN(A22) -FIND("=",A22,15)+2)</f>
-        <v xml:space="preserve"> = rgb(88,85,127)</v>
+        <v xml:space="preserve"> = rgb(148,115,80)</v>
       </c>
       <c r="D22" s="5" t="str">
         <f>CONCATENATE(LEFT(A22,12),B22,C22)</f>
-        <v xml:space="preserve">   var. 2 = #58557F = rgb(88,85,127)</v>
+        <v xml:space="preserve">   var. 2 = #947350 = rgb(148,115,80)</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B23" s="2" t="str">
         <f>MID(A23,13,7)</f>
-        <v>#251F6E</v>
+        <v>#804D19</v>
       </c>
       <c r="C23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(37,31,110)</v>
+        <v xml:space="preserve"> = rgb(128,77,25)</v>
       </c>
       <c r="D23" s="5" t="str">
         <f>CONCATENATE(LEFT(A23,12),B23,C23)</f>
-        <v xml:space="preserve">   var. 3 = #251F6E = rgb(37,31,110)</v>
+        <v xml:space="preserve">   var. 3 = #804D19 = rgb(128,77,25)</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B24" s="2" t="str">
         <f>MID(A24,13,7)</f>
-        <v>#938ED5</v>
+        <v>#E2AF7B</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(147,142,213)</v>
+        <v xml:space="preserve"> = rgb(226,175,123)</v>
       </c>
       <c r="D24" s="5" t="str">
         <f>CONCATENATE(LEFT(A24,12),B24,C24)</f>
-        <v xml:space="preserve">   var. 4 = #938ED5 = rgb(147,142,213)</v>
+        <v xml:space="preserve">   var. 4 = #E2AF7B = rgb(226,175,123)</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B25" s="2" t="str">
         <f>MID(A25,13,7)</f>
-        <v>#A5A1D5</v>
+        <v>#E2BD97</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> = rgb(165,161,213)</v>
+        <v xml:space="preserve"> = rgb(226,189,151)</v>
       </c>
       <c r="D25" s="5" t="str">
         <f>CONCATENATE(LEFT(A25,12),B25,C25)</f>
-        <v xml:space="preserve">   var. 5 = #A5A1D5 = rgb(165,161,213)</v>
+        <v xml:space="preserve">   var. 5 = #E2BD97 = rgb(226,189,151)</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1890,87 +1918,87 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B29" s="2" t="str">
         <f>MID(A29,13,7)</f>
-        <v>#8754A3</v>
+        <v>#C5A94D</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" ref="C29:C49" si="2">RIGHT(A29,LEN(A29) -FIND("=",A29,15)+2)</f>
-        <v xml:space="preserve"> = rgb(135,84,163)</v>
+        <v xml:space="preserve"> = rgb(197,169,77)</v>
       </c>
       <c r="D29" s="5" t="str">
         <f>CONCATENATE(LEFT(A29,12),B29,C29)</f>
-        <v xml:space="preserve">   var. 1 = #8754A3 = rgb(135,84,163)</v>
+        <v xml:space="preserve">   var. 1 = #C5A94D = rgb(197,169,77)</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B30" s="2" t="str">
         <f>MID(A30,13,7)</f>
-        <v>#6A4E7A</v>
+        <v>#948450</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(106,78,122)</v>
+        <v xml:space="preserve"> = rgb(148,132,80)</v>
       </c>
       <c r="D30" s="5" t="str">
         <f>CONCATENATE(LEFT(A30,12),B30,C30)</f>
-        <v xml:space="preserve">   var. 2 = #6A4E7A = rgb(106,78,122)</v>
+        <v xml:space="preserve">   var. 2 = #948450 = rgb(148,132,80)</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B31" s="2" t="str">
         <f>MID(A31,13,7)</f>
-        <v>#4E1B6A</v>
+        <v>#806819</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(78,27,106)</v>
+        <v xml:space="preserve"> = rgb(128,104,25)</v>
       </c>
       <c r="D31" s="5" t="str">
         <f>CONCATENATE(LEFT(A31,12),B31,C31)</f>
-        <v xml:space="preserve">   var. 3 = #4E1B6A = rgb(78,27,106)</v>
+        <v xml:space="preserve">   var. 3 = #806819 = rgb(128,104,25)</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B32" s="2" t="str">
         <f>MID(A32,13,7)</f>
-        <v>#B685D1</v>
+        <v>#E2C97B</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(182,133,209)</v>
+        <v xml:space="preserve"> = rgb(226,201,123)</v>
       </c>
       <c r="D32" s="5" t="str">
         <f>CONCATENATE(LEFT(A32,12),B32,C32)</f>
-        <v xml:space="preserve">   var. 4 = #B685D1 = rgb(182,133,209)</v>
+        <v xml:space="preserve">   var. 4 = #E2C97B = rgb(226,201,123)</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B33" s="2" t="str">
         <f>MID(A33,13,7)</f>
-        <v>#BD99D1</v>
+        <v>#E2D097</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(189,153,209)</v>
+        <v xml:space="preserve"> = rgb(226,208,151)</v>
       </c>
       <c r="D33" s="5" t="str">
         <f>CONCATENATE(LEFT(A33,12),B33,C33)</f>
-        <v xml:space="preserve">   var. 5 = #BD99D1 = rgb(189,153,209)</v>
+        <v xml:space="preserve">   var. 5 = #E2D097 = rgb(226,208,151)</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1995,87 +2023,87 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B37" s="2" t="str">
         <f>MID(A37,13,7)</f>
-        <v>#4E8499</v>
+        <v>#BD4A58</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" ref="C37" si="3">RIGHT(A37,LEN(A37) -FIND("=",A37,15)+2)</f>
-        <v xml:space="preserve"> = rgb(78,132,153)</v>
+        <v xml:space="preserve"> = rgb(189,74,88)</v>
       </c>
       <c r="D37" s="5" t="str">
         <f>CONCATENATE(LEFT(A37,12),B37,C37)</f>
-        <v xml:space="preserve">   var. 1 = #4E8499 = rgb(78,132,153)</v>
+        <v xml:space="preserve">   var. 1 = #BD4A58 = rgb(189,74,88)</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B38" s="2" t="str">
         <f>MID(A38,13,7)</f>
-        <v>#496773</v>
+        <v>#8E4D55</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(73,103,115)</v>
+        <v xml:space="preserve"> = rgb(142,77,85)</v>
       </c>
       <c r="D38" s="5" t="str">
         <f>CONCATENATE(LEFT(A38,12),B38,C38)</f>
-        <v xml:space="preserve">   var. 2 = #496773 = rgb(73,103,115)</v>
+        <v xml:space="preserve">   var. 2 = #8E4D55 = rgb(142,77,85)</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2" t="str">
         <f>MID(A39,13,7)</f>
-        <v>#194F64</v>
+        <v>#7B1824</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(25,79,100)</v>
+        <v xml:space="preserve"> = rgb(123,24,36)</v>
       </c>
       <c r="D39" s="5" t="str">
         <f>CONCATENATE(LEFT(A39,12),B39,C39)</f>
-        <v xml:space="preserve">   var. 3 = #194F64 = rgb(25,79,100)</v>
+        <v xml:space="preserve">   var. 3 = #7B1824 = rgb(123,24,36)</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B40" s="2" t="str">
         <f>MID(A40,13,7)</f>
-        <v>#81B7CC</v>
+        <v>#DE7985</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(129,183,204)</v>
+        <v xml:space="preserve"> = rgb(222,121,133)</v>
       </c>
       <c r="D40" s="5" t="str">
         <f>CONCATENATE(LEFT(A40,12),B40,C40)</f>
-        <v xml:space="preserve">   var. 4 = #81B7CC = rgb(129,183,204)</v>
+        <v xml:space="preserve">   var. 4 = #DE7985 = rgb(222,121,133)</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B41" s="2" t="str">
         <f>MID(A41,13,7)</f>
-        <v>#95BDCC</v>
+        <v>#DE949D</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(149,189,204)</v>
+        <v xml:space="preserve"> = rgb(222,148,157)</v>
       </c>
       <c r="D41" s="5" t="str">
         <f>CONCATENATE(LEFT(A41,12),B41,C41)</f>
-        <v xml:space="preserve">   var. 5 = #95BDCC = rgb(149,189,204)</v>
+        <v xml:space="preserve">   var. 5 = #DE949D = rgb(222,148,157)</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2100,87 +2128,87 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B45" s="2" t="str">
         <f>MID(A45,13,7)</f>
-        <v>#F4D777</v>
+        <v>#336B7B</v>
       </c>
       <c r="C45" s="2" t="str">
         <f t="shared" ref="C45" si="4">RIGHT(A45,LEN(A45) -FIND("=",A45,15)+2)</f>
-        <v xml:space="preserve"> = rgb(244,215,119)</v>
+        <v xml:space="preserve"> = rgb(51,107,123)</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>CONCATENATE(LEFT(A45,12),B45,C45)</f>
-        <v xml:space="preserve">   var. 1 = #F4D777 = rgb(244,215,119)</v>
+        <v xml:space="preserve">   var. 1 = #336B7B = rgb(51,107,123)</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B46" s="2" t="str">
         <f>MID(A46,13,7)</f>
-        <v>#B7A771</v>
+        <v>#33535C</v>
       </c>
       <c r="C46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(183,167,113)</v>
+        <v xml:space="preserve"> = rgb(51,83,92)</v>
       </c>
       <c r="D46" s="5" t="str">
         <f>CONCATENATE(LEFT(A46,12),B46,C46)</f>
-        <v xml:space="preserve">   var. 2 = #B7A771 = rgb(183,167,113)</v>
+        <v xml:space="preserve">   var. 2 = #33535C = rgb(51,83,92)</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B47" s="2" t="str">
         <f>MID(A47,13,7)</f>
-        <v>#9F8327</v>
+        <v>#104250</v>
       </c>
       <c r="C47" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(159,131,39)</v>
+        <v xml:space="preserve"> = rgb(16,66,80)</v>
       </c>
       <c r="D47" s="5" t="str">
         <f>CONCATENATE(LEFT(A47,12),B47,C47)</f>
-        <v xml:space="preserve">   var. 3 = #9F8327 = rgb(159,131,39)</v>
+        <v xml:space="preserve">   var. 3 = #104250 = rgb(16,66,80)</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B48" s="2" t="str">
         <f>MID(A48,13,7)</f>
-        <v>#FAE49A</v>
+        <v>#6AABBD</v>
       </c>
       <c r="C48" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(250,228,154)</v>
+        <v xml:space="preserve"> = rgb(106,171,189)</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>CONCATENATE(LEFT(A48,12),B48,C48)</f>
-        <v xml:space="preserve">   var. 4 = #FAE49A = rgb(250,228,154)</v>
+        <v xml:space="preserve">   var. 4 = #6AABBD = rgb(106,171,189)</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B49" s="2" t="str">
         <f>MID(A49,13,7)</f>
-        <v>#FAE9B3</v>
+        <v>#80AFBD</v>
       </c>
       <c r="C49" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> = rgb(250,233,179)</v>
+        <v xml:space="preserve"> = rgb(128,175,189)</v>
       </c>
       <c r="D49" s="5" t="str">
         <f>CONCATENATE(LEFT(A49,12),B49,C49)</f>
-        <v xml:space="preserve">   var. 5 = #FAE9B3 = rgb(250,233,179)</v>
+        <v xml:space="preserve">   var. 5 = #80AFBD = rgb(128,175,189)</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2295,7 +2323,7 @@
       <c r="C65" s="2"/>
       <c r="D65" s="5" t="str">
         <f>CONCATENATE("a:visited { border-bottom-color: ", B21,"; }")</f>
-        <v>a:visited { border-bottom-color: #645FAA; }</v>
+        <v>a:visited { border-bottom-color: #C58A4D; }</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2334,7 +2362,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="5" t="str">
         <f>CONCATENATE("  color: ", B21,";")</f>
-        <v xml:space="preserve">  color: #645FAA;</v>
+        <v xml:space="preserve">  color: #C58A4D;</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2343,7 +2371,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="5" t="str">
         <f>CONCATENATE("  border-bottom: 1px solid ",B21,";")</f>
-        <v xml:space="preserve">  border-bottom: 1px solid #645FAA;</v>
+        <v xml:space="preserve">  border-bottom: 1px solid #C58A4D;</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2384,14 +2412,14 @@
       <c r="A77" s="2"/>
       <c r="D77" s="5" t="str">
         <f>CONCATENATE("        color:",B21,";")</f>
-        <v xml:space="preserve">        color:#645FAA;</v>
+        <v xml:space="preserve">        color:#C58A4D;</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2"/>
       <c r="D78" s="5" t="str">
         <f>CONCATENATE("        border-bottom: 3px double ", B21,";")</f>
-        <v xml:space="preserve">        border-bottom: 3px double #645FAA;</v>
+        <v xml:space="preserve">        border-bottom: 3px double #C58A4D;</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2412,7 +2440,7 @@
       <c r="A82" s="2"/>
       <c r="D82" s="5" t="str">
         <f>CONCATENATE("a:link { color: ", B31,"; }")</f>
-        <v>a:link { color: #4E1B6A; }</v>
+        <v>a:link { color: #806819; }</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2435,7 +2463,7 @@
       <c r="A86" s="2"/>
       <c r="D86" s="5" t="str">
         <f>CONCATENATE("a:active { color: ", B39,"; }")</f>
-        <v>a:active { color: #194F64; }</v>
+        <v>a:active { color: #7B1824; }</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2446,7 +2474,7 @@
       <c r="A88" s="2"/>
       <c r="D88" s="5" t="str">
         <f>CONCATENATE("a.special { background-color: ",B41,"; }")</f>
-        <v>a.special { background-color: #95BDCC; }</v>
+        <v>a.special { background-color: #DE949D; }</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2477,7 +2505,7 @@
       <c r="A94" s="2"/>
       <c r="D94" s="5" t="str">
         <f>CONCATENATE("h1 { color: ",B21,"; }")</f>
-        <v>h1 { color: #645FAA; }</v>
+        <v>h1 { color: #C58A4D; }</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2488,7 +2516,7 @@
       <c r="A96" s="2"/>
       <c r="D96" s="5" t="str">
         <f>CONCATENATE("h2 { color: ", B46,"; }")</f>
-        <v>h2 { color: #B7A771; }</v>
+        <v>h2 { color: #33535C; }</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2571,7 +2599,7 @@
       <c r="A110" s="2"/>
       <c r="D110" s="5" t="str">
         <f>CONCATENATE("        border-bottom-color: ", B21,";")</f>
-        <v xml:space="preserve">        border-bottom-color: #645FAA;</v>
+        <v xml:space="preserve">        border-bottom-color: #C58A4D;</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2597,8 +2625,8 @@
     <row r="115" spans="1:5">
       <c r="A115" s="2"/>
       <c r="D115" s="5" t="str">
-        <f>CONCATENATE("th { background-color: ", Primary5,"; }")</f>
-        <v>th { background-color: #A5A1D5; }</v>
+        <f>CONCATENATE("th { background-color: ", Primary4,"; }")</f>
+        <v>th { background-color: #E2AF7B; }</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2629,7 +2657,7 @@
       <c r="A120" s="2"/>
       <c r="D120" s="5" t="str">
         <f>CONCATENATE("border-color: ", B22,"; /* P2 */")</f>
-        <v>border-color: #58557F; /* P2 */</v>
+        <v>border-color: #947350; /* P2 */</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>43</v>
@@ -2639,7 +2667,7 @@
       <c r="A121" s="2"/>
       <c r="D121" s="5" t="str">
         <f>CONCATENATE("background-color: ", B21,"; /* colour P1 */")</f>
-        <v>background-color: #645FAA; /* colour P1 */</v>
+        <v>background-color: #C58A4D; /* colour P1 */</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>44</v>
@@ -2649,55 +2677,55 @@
       <c r="A122" s="2"/>
       <c r="D122" s="5" t="str">
         <f>CONCATENATE("background-image: -moz-linear-gradient(top, ",B24," , ", B21, ");")</f>
-        <v>background-image: -moz-linear-gradient(top, #938ED5 , #645FAA);</v>
+        <v>background-image: -moz-linear-gradient(top, #E2AF7B , #C58A4D);</v>
       </c>
       <c r="E122" s="1" t="str">
         <f>CONCATENATE("    text-shadow: ",B23," 1px 1px;")</f>
-        <v xml:space="preserve">    text-shadow: #251F6E 1px 1px;</v>
+        <v xml:space="preserve">    text-shadow: #804D19 1px 1px;</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="16">
       <c r="A123" s="2"/>
       <c r="D123" s="5" t="str">
         <f>CONCATENATE("background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, ", B24, "),color-stop(1, ", B21,"));")</f>
-        <v>background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #938ED5),color-stop(1, #645FAA));</v>
+        <v>background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #E2AF7B),color-stop(1, #C58A4D));</v>
       </c>
       <c r="E123" s="1" t="str">
         <f>CONCATENATE("    border-top: 1px solid ", B25,"; ")</f>
-        <v xml:space="preserve">    border-top: 1px solid #A5A1D5; </v>
+        <v xml:space="preserve">    border-top: 1px solid #E2BD97; </v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="16">
       <c r="A124" s="2"/>
       <c r="D124" s="5" t="str">
         <f>CONCATENATE("background-image: -webkit-linear-gradient(", B24,", ", B21,");")</f>
-        <v>background-image: -webkit-linear-gradient(#938ED5, #645FAA);</v>
+        <v>background-image: -webkit-linear-gradient(#E2AF7B, #C58A4D);</v>
       </c>
       <c r="E124" s="1" t="str">
         <f>CONCATENATE("    border-left: 1px solid ",B25,";")</f>
-        <v xml:space="preserve">    border-left: 1px solid #A5A1D5;</v>
+        <v xml:space="preserve">    border-left: 1px solid #E2BD97;</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="16">
       <c r="A125" s="2"/>
       <c r="D125" s="5" t="str">
         <f>CONCATENATE("background-image: linear-gradient(top, ", B24,", ", B21,");")</f>
-        <v>background-image: linear-gradient(top, #938ED5, #645FAA);</v>
+        <v>background-image: linear-gradient(top, #E2AF7B, #C58A4D);</v>
       </c>
       <c r="E125" s="1" t="str">
         <f>CONCATENATE("    border-right: 1px solid ", B23,";")</f>
-        <v xml:space="preserve">    border-right: 1px solid #251F6E;</v>
+        <v xml:space="preserve">    border-right: 1px solid #804D19;</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="16">
       <c r="A126" s="2"/>
       <c r="D126" s="5" t="str">
         <f>CONCATENATE("filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='", B24, "', EndColorStr='", B21,"');")</f>
-        <v>filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#938ED5', EndColorStr='#645FAA');</v>
+        <v>filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#E2AF7B', EndColorStr='#C58A4D');</v>
       </c>
       <c r="E126" s="1" t="str">
         <f>CONCATENATE("    border-bottom: 1px solid ",B23,";")</f>
-        <v xml:space="preserve">    border-bottom: 1px solid #251F6E;</v>
+        <v xml:space="preserve">    border-bottom: 1px solid #804D19;</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="16">
@@ -2716,7 +2744,7 @@
       </c>
       <c r="E128" s="1" t="str">
         <f>CONCATENATE("        background-image: -moz-linear-gradient(top, ", B21,", ",B22,");")</f>
-        <v xml:space="preserve">        background-image: -moz-linear-gradient(top, #645FAA, #58557F);</v>
+        <v xml:space="preserve">        background-image: -moz-linear-gradient(top, #C58A4D, #947350);</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="16">
@@ -2726,7 +2754,7 @@
       </c>
       <c r="E129" s="1" t="str">
         <f>CONCATENATE("    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, ",B22,"));")</f>
-        <v xml:space="preserve">    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, #58557F));</v>
+        <v xml:space="preserve">    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #ccc),color-stop(1, #947350));</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="16">
@@ -2734,7 +2762,7 @@
       <c r="D130" s="5"/>
       <c r="E130" s="1" t="str">
         <f>CONCATENATE("    background-image: -webkit-linear-gradient(",B21,", ",B22,");" )</f>
-        <v xml:space="preserve">    background-image: -webkit-linear-gradient(#645FAA, #58557F);</v>
+        <v xml:space="preserve">    background-image: -webkit-linear-gradient(#C58A4D, #947350);</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="16">
@@ -2744,7 +2772,7 @@
       </c>
       <c r="E131" s="1" t="str">
         <f>CONCATENATE("    background-image: linear-gradient(top, ", B21, ", ", B22, ");")</f>
-        <v xml:space="preserve">    background-image: linear-gradient(top, #645FAA, #58557F);</v>
+        <v xml:space="preserve">    background-image: linear-gradient(top, #C58A4D, #947350);</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="16">
@@ -2754,14 +2782,14 @@
       </c>
       <c r="E132" s="1" t="str">
         <f>CONCATENATE("    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='", B21, "', EndColorStr='", B22,"');")</f>
-        <v xml:space="preserve">    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#645FAA', EndColorStr='#58557F');</v>
+        <v xml:space="preserve">    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#C58A4D', EndColorStr='#947350');</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="16">
       <c r="A133" s="2"/>
       <c r="D133" s="5" t="str">
         <f>CONCATENATE("form input.submit:active { background: ", B21,"; }")</f>
-        <v>form input.submit:active { background: #645FAA; }</v>
+        <v>form input.submit:active { background: #C58A4D; }</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>22</v>
@@ -2775,7 +2803,7 @@
       <c r="A135" s="2"/>
       <c r="D135" s="5" t="str">
         <f>CONCATENATE("div.box { border: 10px solid ", SECB5,"; }")</f>
-        <v>div.box { border: 10px solid #95BDCC; }</v>
+        <v>div.box { border: 10px solid #DE949D; }</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>46</v>
@@ -2786,14 +2814,13 @@
       <c r="D136" s="5"/>
       <c r="E136" s="1" t="str">
         <f>CONCATENATE("div#local-masthead { background-color: ", B25, "; }")</f>
-        <v>div#local-masthead { background-color: #A5A1D5; }</v>
+        <v>div#local-masthead { background-color: #E2BD97; }</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="2"/>
-      <c r="D137" s="5" t="str">
-        <f>CONCATENATE("div#local-masthead { background-color: ", B25,"; }")</f>
-        <v>div#local-masthead { background-color: #A5A1D5; }</v>
+      <c r="D137" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="16">
@@ -2805,8 +2832,9 @@
     </row>
     <row r="139" spans="1:5" ht="16">
       <c r="A139" s="2"/>
-      <c r="D139" s="5" t="s">
-        <v>47</v>
+      <c r="D139" s="5" t="str">
+        <f>CONCATENATE("    background-color: ", Primary5,";")</f>
+        <v xml:space="preserve">    background-color: #E2BD97;</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>48</v>
@@ -2814,8 +2842,9 @@
     </row>
     <row r="140" spans="1:5" ht="16">
       <c r="A140" s="2"/>
-      <c r="D140" s="5" t="s">
-        <v>48</v>
+      <c r="D140" s="5" t="str">
+        <f>CONCATENATE("    background-image: -moz-linear-gradient(top, ", Primary5, ", ",Primary1,");")</f>
+        <v xml:space="preserve">    background-image: -moz-linear-gradient(top, #E2BD97, #C58A4D);</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>49</v>
@@ -2823,8 +2852,9 @@
     </row>
     <row r="141" spans="1:5" ht="16">
       <c r="A141" s="2"/>
-      <c r="D141" s="5" t="s">
-        <v>49</v>
+      <c r="D141" s="5" t="str">
+        <f>CONCATENATE("    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, ", Primary5,"),color-stop(1, ", Primary1,"));")</f>
+        <v xml:space="preserve">    background-image: -webkit-gradient(linear,left top,left bottom,color-stop(0, #E2BD97),color-stop(1, #C58A4D));</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>50</v>
@@ -2832,19 +2862,20 @@
     </row>
     <row r="142" spans="1:5" ht="16">
       <c r="A142" s="2"/>
-      <c r="D142" s="5" t="s">
-        <v>50</v>
+      <c r="D142" s="5" t="str">
+        <f>CONCATENATE("    background-image: -webkit-linear-gradient(", Primary5,", ", Primary1,");")</f>
+        <v xml:space="preserve">    background-image: -webkit-linear-gradient(#E2BD97, #C58A4D);</v>
       </c>
       <c r="E142" s="1" t="str">
         <f>CONCATENATE("border-bottom: 3px solid ", B21, ";")</f>
-        <v>border-bottom: 3px solid #645FAA;</v>
+        <v>border-bottom: 3px solid #C58A4D;</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="16">
       <c r="A143" s="2"/>
       <c r="D143" s="5" t="str">
-        <f>CONCATENATE("border-bottom: 3px solid ", Primary1, ";")</f>
-        <v>border-bottom: 3px solid #645FAA;</v>
+        <f>CONCATENATE("    background-image: linear-gradient(top, ", Primary5, ", ", Primary1, ");")</f>
+        <v xml:space="preserve">    background-image: linear-gradient(top, #E2BD97, #C58A4D);</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>22</v>
@@ -2852,18 +2883,24 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="2"/>
-      <c r="D144" s="5" t="s">
-        <v>22</v>
+      <c r="D144" s="5" t="str">
+        <f>CONCATENATE("    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='", Primary5,"', EndColorStr='", Primary1,"'); /* IE6/7 */")</f>
+        <v xml:space="preserve">    filter: progid:DXImageTransform.Microsoft.gradient(startColorStr='#E2BD97', EndColorStr='#C58A4D'); /* IE6/7 */</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="2"/>
-      <c r="D145" s="5"/>
+      <c r="D145" s="5" t="str">
+        <f>CONCATENATE("    -ms-filter: ""progid:DXImageTransform.Microsoft.gradient(startColorStr='", Primary5, "', EndColorStr='", Primary1,"')""; /* IE8*/")</f>
+        <v xml:space="preserve">    -ms-filter: "progid:DXImageTransform.Microsoft.gradient(startColorStr='#E2BD97', EndColorStr='#C58A4D')"; /* IE8*/</v>
+      </c>
       <c r="E145" s="3"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="2"/>
-      <c r="D146" s="5"/>
+      <c r="D146" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E146" s="3"/>
     </row>
     <row r="147" spans="1:5">
@@ -2873,51 +2910,54 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="2"/>
-      <c r="D148" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="D148" s="5"/>
       <c r="E148" s="3"/>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="2"/>
       <c r="D149" s="5" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E149" s="3"/>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="2"/>
-      <c r="D150" s="5"/>
+      <c r="D150" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="2"/>
       <c r="D151" s="5" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E151" s="3"/>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="2"/>
-      <c r="D152" s="5"/>
+      <c r="D152" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E152" s="3"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="2"/>
-      <c r="D153" s="5"/>
+      <c r="D153" s="5" t="str">
+        <f>CONCATENATE("border-bottom: 3px solid ", Primary1, ";")</f>
+        <v>border-bottom: 3px solid #C58A4D;</v>
+      </c>
       <c r="E153" s="3"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="2"/>
       <c r="D154" s="5" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="E154" s="3"/>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="2"/>
-      <c r="D155" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="D155" s="5"/>
       <c r="E155" s="3"/>
     </row>
     <row r="156" spans="1:5">
@@ -2926,198 +2966,238 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="2"/>
-      <c r="D157" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="D157" s="5"/>
       <c r="E157" s="3"/>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="2"/>
-      <c r="D158" s="5"/>
+      <c r="D158" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E158" s="3"/>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="2"/>
-      <c r="D159" s="5"/>
+      <c r="D159" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E159" s="3"/>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="2"/>
-      <c r="D160" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="D160" s="5"/>
       <c r="E160" s="3"/>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="2"/>
-      <c r="D161" s="5"/>
+      <c r="D161" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E161" s="3"/>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="2"/>
-      <c r="D162" s="5" t="str">
-        <f>CONCATENATE(".primary-1 { background-color: ", Primary1,"}")</f>
-        <v>.primary-1 { background-color: #645FAA}</v>
-      </c>
+      <c r="D162" s="5"/>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="2"/>
-      <c r="D163" s="5" t="str">
-        <f>CONCATENATE(".primary-2 { background-color: ", Primary2,"}")</f>
-        <v>.primary-2 { background-color: #58557F}</v>
-      </c>
+      <c r="D163" s="5"/>
       <c r="E163" s="3"/>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="2"/>
-      <c r="D164" s="5" t="str">
-        <f>CONCATENATE(".primary-3 { background-color: ", Primary3,"}")</f>
-        <v>.primary-3 { background-color: #251F6E}</v>
+      <c r="D164" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E164" s="3"/>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="2"/>
-      <c r="D165" s="5" t="str">
-        <f>CONCATENATE(".primary-4 { background-color: ", Primary4,"}")</f>
-        <v>.primary-4 { background-color: #938ED5}</v>
+      <c r="D165" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="E165" s="3"/>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="2"/>
-      <c r="D166" s="5" t="str">
-        <f>CONCATENATE(".primary-5 { background-color: ", Primary5,"}")</f>
-        <v>.primary-5 { background-color: #A5A1D5}</v>
-      </c>
+      <c r="D166" s="5"/>
       <c r="E166" s="3"/>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="2"/>
-      <c r="D167" s="5"/>
+      <c r="D167" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="E167" s="3"/>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="2"/>
-      <c r="D168" s="5" t="str">
-        <f>CONCATENATE(".secondary-a-1 { background-color: ", SECA1,"}")</f>
-        <v>.secondary-a-1 { background-color: #8754A3}</v>
-      </c>
+      <c r="D168" s="5"/>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="2"/>
-      <c r="D169" s="5" t="str">
-        <f>CONCATENATE(".secondary-a-2 { background-color: ", SECA2,"}")</f>
-        <v>.secondary-a-2 { background-color: #6A4E7A}</v>
-      </c>
+      <c r="D169" s="5"/>
       <c r="E169" s="4"/>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="2"/>
-      <c r="D170" s="5" t="str">
-        <f>CONCATENATE(".secondary-a-3 { background-color: ", SECA3,"}")</f>
-        <v>.secondary-a-3 { background-color: #4E1B6A}</v>
+      <c r="D170" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="2"/>
-      <c r="D171" s="5" t="str">
-        <f>CONCATENATE(".secondary-a-4 { background-color: ", SECA4,"}")</f>
-        <v>.secondary-a-4 { background-color: #B685D1}</v>
-      </c>
+      <c r="D171" s="5"/>
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="2"/>
       <c r="D172" s="5" t="str">
-        <f>CONCATENATE(".secondary-a-5 { background-color: ", SECA5,"}")</f>
-        <v>.secondary-a-5 { background-color: #BD99D1}</v>
+        <f>CONCATENATE(".primary-1 { background-color: ", Primary1,"}")</f>
+        <v>.primary-1 { background-color: #C58A4D}</v>
       </c>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="2"/>
-      <c r="D173" s="5"/>
+      <c r="D173" s="5" t="str">
+        <f>CONCATENATE(".primary-2 { background-color: ", Primary2,"}")</f>
+        <v>.primary-2 { background-color: #947350}</v>
+      </c>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="2"/>
       <c r="D174" s="5" t="str">
-        <f>CONCATENATE(".secondary-b-1 { background-color: ", SECB1,"}")</f>
-        <v>.secondary-b-1 { background-color: #4E8499}</v>
+        <f>CONCATENATE(".primary-3 { background-color: ", Primary3,"}")</f>
+        <v>.primary-3 { background-color: #804D19}</v>
       </c>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="2"/>
       <c r="D175" s="5" t="str">
-        <f>CONCATENATE(".secondary-b-2 { background-color: ", SECB2,"}")</f>
-        <v>.secondary-b-2 { background-color: #496773}</v>
+        <f>CONCATENATE(".primary-4 { background-color: ", Primary4,"}")</f>
+        <v>.primary-4 { background-color: #E2AF7B}</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="2"/>
       <c r="D176" s="5" t="str">
-        <f>CONCATENATE(".secondary-b-3 { background-color: ", SECB3,"}")</f>
-        <v>.secondary-b-3 { background-color: #194F64}</v>
+        <f>CONCATENATE(".primary-5 { background-color: ", Primary5,"}")</f>
+        <v>.primary-5 { background-color: #E2BD97}</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="2"/>
-      <c r="D177" s="5" t="str">
-        <f>CONCATENATE(".secondary-b-4 { background-color: ", SECB4,"}")</f>
-        <v>.secondary-b-4 { background-color: #81B7CC}</v>
-      </c>
+      <c r="D177" s="5"/>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="2"/>
       <c r="D178" s="5" t="str">
-        <f>CONCATENATE(".secondary-b-5 { background-color: ", SECB5,"}")</f>
-        <v>.secondary-b-5 { background-color: #95BDCC}</v>
+        <f>CONCATENATE(".secondary-a-1 { background-color: ", SECA1,"}")</f>
+        <v>.secondary-a-1 { background-color: #C5A94D}</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="2"/>
-      <c r="D179" s="5"/>
+      <c r="D179" s="5" t="str">
+        <f>CONCATENATE(".secondary-a-2 { background-color: ", SECA2,"}")</f>
+        <v>.secondary-a-2 { background-color: #948450}</v>
+      </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="2"/>
       <c r="D180" s="5" t="str">
-        <f>CONCATENATE(".complement-1 { background-color: ", COMP1,"}")</f>
-        <v>.complement-1 { background-color: #F4D777}</v>
+        <f>CONCATENATE(".secondary-a-3 { background-color: ", SECA3,"}")</f>
+        <v>.secondary-a-3 { background-color: #806819}</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="2"/>
       <c r="D181" s="5" t="str">
-        <f>CONCATENATE(".complement-2 { background-color: ", COMP2,"}")</f>
-        <v>.complement-2 { background-color: #B7A771}</v>
+        <f>CONCATENATE(".secondary-a-4 { background-color: ", SECA4,"}")</f>
+        <v>.secondary-a-4 { background-color: #E2C97B}</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="2"/>
       <c r="D182" s="5" t="str">
-        <f>CONCATENATE(".complement-3 { background-color: ", COMP3,"}")</f>
-        <v>.complement-3 { background-color: #9F8327}</v>
+        <f>CONCATENATE(".secondary-a-5 { background-color: ", SECA5,"}")</f>
+        <v>.secondary-a-5 { background-color: #E2D097}</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="2"/>
-      <c r="D183" s="5" t="str">
-        <f>CONCATENATE(".complement-4 { background-color: ", COMP4,"}")</f>
-        <v>.complement-4 { background-color: #FAE49A}</v>
-      </c>
+      <c r="D183" s="5"/>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="2"/>
       <c r="D184" s="5" t="str">
-        <f>CONCATENATE(".complement-5 { background-color: ", COMP5,"}")</f>
-        <v>.complement-5 { background-color: #FAE9B3}</v>
+        <f>CONCATENATE(".secondary-b-1 { background-color: ", SECB1,"}")</f>
+        <v>.secondary-b-1 { background-color: #BD4A58}</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="2"/>
-      <c r="D185" s="5"/>
+      <c r="D185" s="5" t="str">
+        <f>CONCATENATE(".secondary-b-2 { background-color: ", SECB2,"}")</f>
+        <v>.secondary-b-2 { background-color: #8E4D55}</v>
+      </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="2"/>
-      <c r="D186" s="5" t="s">
+      <c r="D186" s="5" t="str">
+        <f>CONCATENATE(".secondary-b-3 { background-color: ", SECB3,"}")</f>
+        <v>.secondary-b-3 { background-color: #7B1824}</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="D187" s="5" t="str">
+        <f>CONCATENATE(".secondary-b-4 { background-color: ", SECB4,"}")</f>
+        <v>.secondary-b-4 { background-color: #DE7985}</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="D188" s="5" t="str">
+        <f>CONCATENATE(".secondary-b-5 { background-color: ", SECB5,"}")</f>
+        <v>.secondary-b-5 { background-color: #DE949D}</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="D190" s="5" t="str">
+        <f>CONCATENATE(".complement-1 { background-color: ", COMP1,"}")</f>
+        <v>.complement-1 { background-color: #336B7B}</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="D191" s="5" t="str">
+        <f>CONCATENATE(".complement-2 { background-color: ", COMP2,"}")</f>
+        <v>.complement-2 { background-color: #33535C}</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="D192" s="5" t="str">
+        <f>CONCATENATE(".complement-3 { background-color: ", COMP3,"}")</f>
+        <v>.complement-3 { background-color: #104250}</v>
+      </c>
+    </row>
+    <row r="193" spans="4:4">
+      <c r="D193" s="5" t="str">
+        <f>CONCATENATE(".complement-4 { background-color: ", COMP4,"}")</f>
+        <v>.complement-4 { background-color: #6AABBD}</v>
+      </c>
+    </row>
+    <row r="194" spans="4:4">
+      <c r="D194" s="5" t="str">
+        <f>CONCATENATE(".complement-5 { background-color: ", COMP5,"}")</f>
+        <v>.complement-5 { background-color: #80AFBD}</v>
+      </c>
+    </row>
+    <row r="195" spans="4:4">
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="4:4">
+      <c r="D196" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3137,10 +3217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C340"/>
+  <dimension ref="A1:C344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="A342" sqref="A342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3595,14 +3675,14 @@
       <c r="A85" s="9"/>
       <c r="B85" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #251F6E;</v>
+        <v>color: #804D19;</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="9"/>
       <c r="B86" s="9" t="str">
         <f>CONCATENATE("background: ", Primary4,";")</f>
-        <v>background: #938ED5;</v>
+        <v>background: #E2AF7B;</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3875,8 +3955,8 @@
     </row>
     <row r="149" spans="1:2">
       <c r="B149" s="7" t="str">
-        <f>CONCATENATE("color:",COMP1,";")</f>
-        <v>color:#F4D777;</v>
+        <f>CONCATENATE("color:",SECA4,";")</f>
+        <v>color:#E2C97B;</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -3901,8 +3981,8 @@
     </row>
     <row r="155" spans="1:2">
       <c r="B155" s="7" t="str">
-        <f>CONCATENATE("background-color:", COMP1,";")</f>
-        <v>background-color:#F4D777;</v>
+        <f>CONCATENATE("background-color:", SECA4,";")</f>
+        <v>background-color:#E2C97B;</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -3917,8 +3997,8 @@
     </row>
     <row r="159" spans="1:2">
       <c r="B159" s="7" t="str">
-        <f>CONCATENATE("color:", SECB1, ";")</f>
-        <v>color:#4E8499;</v>
+        <f>CONCATENATE("color:", SECB4, ";")</f>
+        <v>color:#DE7985;</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -3938,8 +4018,8 @@
     </row>
     <row r="164" spans="1:2">
       <c r="B164" s="7" t="str">
-        <f>CONCATENATE("background-color:", SECB1, ";")</f>
-        <v>background-color:#4E8499;</v>
+        <f>CONCATENATE("background-color:", SECB4, ";")</f>
+        <v>background-color:#DE7985;</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -4225,7 +4305,7 @@
     <row r="231" spans="1:2">
       <c r="B231" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #251F6E;</v>
+        <v>color: #804D19;</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -4266,7 +4346,7 @@
     <row r="240" spans="1:2">
       <c r="B240" s="7" t="str">
         <f>CONCATENATE("color: ", COMP3,";")</f>
-        <v>color: #9F8327;</v>
+        <v>color: #104250;</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -4302,7 +4382,7 @@
     <row r="248" spans="1:2">
       <c r="B248" s="7" t="str">
         <f>CONCATENATE("border: 1px solid ", Primary3)</f>
-        <v>border: 1px solid #251F6E</v>
+        <v>border: 1px solid #804D19</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -4358,7 +4438,7 @@
     <row r="260" spans="1:2">
       <c r="B260" s="7" t="str">
         <f>CONCATENATE("background: ", Primary5, ";")</f>
-        <v>background: #A5A1D5;</v>
+        <v>background: #E2BD97;</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -4384,13 +4464,13 @@
     <row r="266" spans="1:2">
       <c r="B266" s="7" t="str">
         <f>CONCATENATE("background: ", Primary4, ";")</f>
-        <v>background: #938ED5;</v>
+        <v>background: #E2AF7B;</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="B267" s="7" t="str">
         <f>CONCATENATE("color: ", Primary3, ";")</f>
-        <v>color: #251F6E;</v>
+        <v>color: #804D19;</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -4426,7 +4506,7 @@
     <row r="275" spans="1:2">
       <c r="B275" s="7" t="str">
         <f>CONCATENATE("border-top-color:", COMP3,";")</f>
-        <v>border-top-color:#9F8327;</v>
+        <v>border-top-color:#104250;</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -4631,8 +4711,8 @@
     </row>
     <row r="324" spans="1:2">
       <c r="B324" s="7" t="str">
-        <f>CONCATENATE("background: ", Primary2,";")</f>
-        <v>background: #58557F;</v>
+        <f>CONCATENATE("background: ", "#e8e8e8",";")</f>
+        <v>background: #e8e8e8;</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -4705,10 +4785,25 @@
         <v>22</v>
       </c>
     </row>
+    <row r="342" spans="1:1">
+      <c r="A342" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1">
+      <c r="A343" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1">
+      <c r="A344" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="J1:J340">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>